<commit_message>
Fixed bug where Excel formula error causes unhandled exception
</commit_message>
<xml_diff>
--- a/LightweightExcelReader.Tests/TestSpreadsheets/TestSpreadsheet1.xlsx
+++ b/LightweightExcelReader.Tests/TestSpreadsheets/TestSpreadsheet1.xlsx
@@ -97,7 +97,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -198,6 +198,78 @@
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>41274</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1.234</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>42286</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>9.876</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="2"/>
+      <c r="D4" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,7 +290,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>1</v>
@@ -232,7 +304,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>2</v>
@@ -245,6 +317,9 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="n">
         <v>5</v>
@@ -253,26 +328,26 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -290,81 +365,6 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>41274</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>1.234</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>42286</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>9.876</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1" t="n">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
@@ -409,7 +409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -419,7 +419,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.6"/>
@@ -497,7 +497,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -507,7 +507,7 @@
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -577,7 +577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -587,7 +587,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -658,7 +658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -668,7 +668,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -681,7 +681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -691,7 +691,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -704,7 +704,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -714,7 +714,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -727,7 +727,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -737,7 +737,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>